<commit_message>
added readme for the program
</commit_message>
<xml_diff>
--- a/project files/Team Intro.xlsx
+++ b/project files/Team Intro.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TheChosenOne\Google Drive\Winter 2016 Concordia University\SOEN 341 Software Process\Project\AnotherOne\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TheChosenOne\Desktop\AnotherOne\project files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19428" windowHeight="3852"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19428" windowHeight="3852" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="49">
   <si>
     <t>Alessandro Power</t>
   </si>
@@ -151,6 +151,27 @@
   </si>
   <si>
     <t>I have rank diamond 1 in LOL and lift 300 pounds.</t>
+  </si>
+  <si>
+    <t>Documentation, Front End</t>
+  </si>
+  <si>
+    <t>Programming: Everything</t>
+  </si>
+  <si>
+    <t>Ronn Pang</t>
+  </si>
+  <si>
+    <t>Programming: Implementation</t>
+  </si>
+  <si>
+    <t>I am still on the waitlist</t>
+  </si>
+  <si>
+    <t>Programming: Database or Documentation</t>
+  </si>
+  <si>
+    <t>Programming but limited; Testing</t>
   </si>
 </sst>
 </file>
@@ -213,11 +234,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -505,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -520,15 +542,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -824,6 +846,32 @@
         <v>29</v>
       </c>
     </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>37</v>
@@ -842,7 +890,7 @@
         <v>34</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -859,7 +907,7 @@
       </c>
       <c r="B21">
         <f>SUM(B18:B20)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -876,14 +924,148 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="25.88671875" customWidth="1"/>
+    <col min="2" max="2" width="39.77734375" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A3:C14">
+    <sortCondition ref="A3"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>